<commit_message>
trying to deploy - issues with kevin's machine and outlook. Added dropdown to wordvb library
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2FEB0C-480D-48CC-A84C-C1EB7BDB84D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A18135-6C4F-47BF-8BCB-4D64B5967E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="19320" windowHeight="9750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>CompanyName</t>
   </si>
   <si>
-    <t>ACompName1</t>
-  </si>
-  <si>
     <t>CompanyAddress</t>
   </si>
   <si>
@@ -273,30 +270,6 @@
     <t>ContactEmail</t>
   </si>
   <si>
-    <t>ACompAddress1</t>
-  </si>
-  <si>
-    <t>ACompPostcode1</t>
-  </si>
-  <si>
-    <t>Acompnameifdiff</t>
-  </si>
-  <si>
-    <t>AAddressIfDiff</t>
-  </si>
-  <si>
-    <t>ApostcodeIfDiff</t>
-  </si>
-  <si>
-    <t>AConName</t>
-  </si>
-  <si>
-    <t>AConTel</t>
-  </si>
-  <si>
-    <t>AConEmail</t>
-  </si>
-  <si>
     <t>ApplicantName</t>
   </si>
   <si>
@@ -306,15 +279,6 @@
     <t>ApplicantCompany</t>
   </si>
   <si>
-    <t>Gcompanyname</t>
-  </si>
-  <si>
-    <t>GPosition</t>
-  </si>
-  <si>
-    <t>GNameBLOCK</t>
-  </si>
-  <si>
     <t>Signature</t>
   </si>
   <si>
@@ -324,18 +288,6 @@
     <t>Spanish</t>
   </si>
   <si>
-    <t>FSpan</t>
-  </si>
-  <si>
-    <t>FEng</t>
-  </si>
-  <si>
-    <t>Fyesorig</t>
-  </si>
-  <si>
-    <t>ESoE</t>
-  </si>
-  <si>
     <t>ScheduleOA</t>
   </si>
   <si>
@@ -408,75 +360,12 @@
     <t>DioxinFree</t>
   </si>
   <si>
-    <t>BDioxFree</t>
-  </si>
-  <si>
-    <t>BNonAn</t>
-  </si>
-  <si>
-    <t>BNonMam</t>
-  </si>
-  <si>
-    <t>BMandFSaleAF</t>
-  </si>
-  <si>
-    <t>BFSaleAF</t>
-  </si>
-  <si>
-    <t>BFSAlc</t>
-  </si>
-  <si>
-    <t>BHumCons</t>
-  </si>
-  <si>
-    <t>BDecOrig</t>
-  </si>
-  <si>
-    <t>BMandFS</t>
-  </si>
-  <si>
-    <t>BFSS</t>
-  </si>
-  <si>
-    <t>CProdname</t>
-  </si>
-  <si>
-    <t>CSepCerts</t>
-  </si>
-  <si>
     <t>Dropdown1</t>
   </si>
   <si>
-    <t>CAddDetails</t>
-  </si>
-  <si>
-    <t>CCosigneeName</t>
-  </si>
-  <si>
-    <t>CDestCount</t>
-  </si>
-  <si>
-    <t>DMandN</t>
-  </si>
-  <si>
-    <t>DNoPack</t>
-  </si>
-  <si>
-    <t>DProdDets</t>
-  </si>
-  <si>
     <t>Dropdown2</t>
   </si>
   <si>
-    <t>DadditionalDeets</t>
-  </si>
-  <si>
-    <t>DCosigneeAdd2</t>
-  </si>
-  <si>
-    <t>DDestinCount</t>
-  </si>
-  <si>
     <t>CountryLookUpPath</t>
   </si>
   <si>
@@ -490,6 +379,117 @@
   </si>
   <si>
     <t>Trader, RPA</t>
+  </si>
+  <si>
+    <t>CompName1</t>
+  </si>
+  <si>
+    <t>CompAddress1</t>
+  </si>
+  <si>
+    <t>CompPostcode1</t>
+  </si>
+  <si>
+    <t>compnameifdiff</t>
+  </si>
+  <si>
+    <t>AddressIfDiff</t>
+  </si>
+  <si>
+    <t>postcodeIfDiff</t>
+  </si>
+  <si>
+    <t>ConName</t>
+  </si>
+  <si>
+    <t>ConTel</t>
+  </si>
+  <si>
+    <t>ConEmail</t>
+  </si>
+  <si>
+    <t>FSS</t>
+  </si>
+  <si>
+    <t>MandFS</t>
+  </si>
+  <si>
+    <t>DecOrig</t>
+  </si>
+  <si>
+    <t>HumCons</t>
+  </si>
+  <si>
+    <t>FSAlc</t>
+  </si>
+  <si>
+    <t>Fsale</t>
+  </si>
+  <si>
+    <t>MandFSale</t>
+  </si>
+  <si>
+    <t>NonMam</t>
+  </si>
+  <si>
+    <t>NonAn</t>
+  </si>
+  <si>
+    <t>DioxFree</t>
+  </si>
+  <si>
+    <t>Prodname</t>
+  </si>
+  <si>
+    <t>SepCerts</t>
+  </si>
+  <si>
+    <t>AddDetails</t>
+  </si>
+  <si>
+    <t>CosigneeName</t>
+  </si>
+  <si>
+    <t>DestCount</t>
+  </si>
+  <si>
+    <t>MandN</t>
+  </si>
+  <si>
+    <t>NoPack</t>
+  </si>
+  <si>
+    <t>ProdDets</t>
+  </si>
+  <si>
+    <t>additionalDeets</t>
+  </si>
+  <si>
+    <t>CosigneeAdd2</t>
+  </si>
+  <si>
+    <t>DestinCount</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>yesorig</t>
+  </si>
+  <si>
+    <t>Eng</t>
+  </si>
+  <si>
+    <t>Span</t>
+  </si>
+  <si>
+    <t>NameBLOCK</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>companyname</t>
   </si>
 </sst>
 </file>
@@ -968,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1187,7 +1187,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>43</v>
@@ -1235,13 +1235,13 @@
     </row>
     <row r="26" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>53</v>
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A44EFD-45F3-423F-B2B0-CF6CEF7186D6}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,80 +1348,80 @@
       <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>70</v>
+      <c r="B3" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="C11" s="7"/>
     </row>
@@ -1429,96 +1429,96 @@
       <c r="A12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>133</v>
+        <v>98</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>132</v>
+        <v>99</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>131</v>
+        <v>100</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>130</v>
+        <v>101</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>129</v>
+        <v>102</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>128</v>
+        <v>103</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>127</v>
+        <v>104</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>126</v>
+        <v>105</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>125</v>
+        <v>106</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>124</v>
+        <v>107</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1526,60 +1526,60 @@
       <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>135</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>136</v>
+        <v>97</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>137</v>
+        <v>96</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>138</v>
+        <v>90</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>139</v>
+        <v>91</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="C29" s="7"/>
     </row>
@@ -1587,69 +1587,69 @@
       <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>140</v>
+        <v>85</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>141</v>
+        <v>86</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>142</v>
+        <v>87</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>143</v>
+        <v>94</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>144</v>
+        <v>95</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>145</v>
+        <v>92</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>146</v>
+        <v>93</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="C37" s="4"/>
     </row>
@@ -1657,15 +1657,15 @@
       <c r="A38" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>99</v>
+        <v>84</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="C39" s="4"/>
     </row>
@@ -1673,33 +1673,33 @@
       <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="7"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>97</v>
+        <v>82</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>96</v>
+        <v>83</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="C43" s="4"/>
     </row>
@@ -1707,33 +1707,33 @@
       <c r="A44" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="7"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>91</v>
+        <v>79</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="C47" s="4"/>
     </row>

</xml_diff>

<commit_message>
Start of sprint 3, added invokes to ProcessChildCase and user detail checks
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A18135-6C4F-47BF-8BCB-4D64B5967E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CF6206-828B-4466-A4F6-84EA1AB9AD54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="19320" windowHeight="9750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="155">
   <si>
     <t>Name</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t>companyname</t>
+  </si>
+  <si>
+    <t>CertificateTemplatesPath</t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\CoFS for G drive\RobotDocuments\Robot Certificate Templates\</t>
+  </si>
+  <si>
+    <t>Folder path for the robot's version of certificate templates</t>
   </si>
 </sst>
 </file>
@@ -646,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C34" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C35" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -966,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,70 +1244,81 @@
     </row>
     <row r="26" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>54</v>
+        <v>114</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1315,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A44EFD-45F3-423F-B2B0-CF6CEF7186D6}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Journey testing bp3, and created user address check workflow
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CF6206-828B-4466-A4F6-84EA1AB9AD54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0FAC2-2DB9-4A37-8FCA-9DEB460B0226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17880" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -499,6 +499,12 @@
   </si>
   <si>
     <t>Folder path for the robot's version of certificate templates</t>
+  </si>
+  <si>
+    <t>BreakoutNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of child cases the robot will run before showing the breakout message. </t>
   </si>
 </sst>
 </file>
@@ -655,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C35" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -975,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,216 +1115,227 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="B13" s="4">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4">
-        <v>1000</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>22</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B16" s="4">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B18" s="4">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4">
+        <v>60000</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B20" s="4">
         <v>120000</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B22" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>153</v>
+        <v>61</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>114</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Address label and entering certificate details
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0FAC2-2DB9-4A37-8FCA-9DEB460B0226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311D9181-9E26-4B75-847F-2BA4A43DAF94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -505,6 +505,15 @@
   </si>
   <si>
     <t xml:space="preserve">Number of child cases the robot will run before showing the breakout message. </t>
+  </si>
+  <si>
+    <t>RobotExceptionFolder</t>
+  </si>
+  <si>
+    <t>\Desktop\RobotWorkingFolder\Exceptions\</t>
+  </si>
+  <si>
+    <t>Folder path for exceptions folder</t>
   </si>
 </sst>
 </file>
@@ -661,8 +670,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C37" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -981,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,94 +1257,105 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>153</v>
+        <v>61</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>114</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed cert counter logic
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311D9181-9E26-4B75-847F-2BA4A43DAF94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45164C32-8237-4C8A-9463-C584F471499E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t>WorkPackageName</t>
   </si>
   <si>
-    <t>CRMInfo</t>
-  </si>
-  <si>
     <t>Certificates-of-Free-Sale</t>
   </si>
   <si>
@@ -514,6 +511,108 @@
   </si>
   <si>
     <t>Folder path for exceptions folder</t>
+  </si>
+  <si>
+    <t>ToBePrintedFolder</t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\COFS to be printed March 2021\Robot\</t>
+  </si>
+  <si>
+    <t>Folder path for the 'to be printed' folder to store finished certificates in.</t>
+  </si>
+  <si>
+    <t>AddressLabelPath</t>
+  </si>
+  <si>
+    <t>\\EARTH.GSI.GOV.UK\USER\SHARED\Agency\CoFS for G drive\RobotDocuments\RobotAddressLabelTemplate.docx</t>
+  </si>
+  <si>
+    <t>CertificatePlaceholders</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>ProductsHere</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>PRODUCERHERE</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>COUNTRYHERE</t>
+  </si>
+  <si>
+    <t>Consignee</t>
+  </si>
+  <si>
+    <t>CONSIGNEEHERE</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>MARKSHERE</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>PACKAGESHERE</t>
+  </si>
+  <si>
+    <t>TRD</t>
+  </si>
+  <si>
+    <t>TRDHERE</t>
+  </si>
+  <si>
+    <t>companyaddresshere</t>
+  </si>
+  <si>
+    <t>ScheduleofAnalysis</t>
+  </si>
+  <si>
+    <t>ScheduleOfAnalysisHere</t>
+  </si>
+  <si>
+    <t>AdditionalHeader</t>
+  </si>
+  <si>
+    <t>AdditionalHeaderHere</t>
+  </si>
+  <si>
+    <t>AdditionalDescription</t>
+  </si>
+  <si>
+    <t>Additionaldescriptionhere</t>
+  </si>
+  <si>
+    <t>AddressLabel</t>
+  </si>
+  <si>
+    <t>AddressLabelHere</t>
+  </si>
+  <si>
+    <t>NumberOfCopies</t>
+  </si>
+  <si>
+    <t>NumberOfCopiesHere</t>
+  </si>
+  <si>
+    <t>SeparateProducts</t>
+  </si>
+  <si>
+    <t>{\Wproduct\W:\W((\w+\s*\W)+)}</t>
+  </si>
+  <si>
+    <t>{\Wproduct\W:\W(\d+\s*)+\W}</t>
   </si>
 </sst>
 </file>
@@ -670,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C37" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C54" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -990,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,10 +1126,10 @@
         <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,13 +1225,13 @@
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1222,10 +1321,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,7 +1339,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>6</v>
@@ -1248,116 +1347,254 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1372,7 +1609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A44EFD-45F3-423F-B2B0-CF6CEF7186D6}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1396,401 +1633,401 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C47" s="4"/>
     </row>

</xml_diff>

<commit_message>
end of sprint 4, full process in live. Added logic for certs requested and breakpoint nos.
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45164C32-8237-4C8A-9463-C584F471499E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20BD4E-A035-4742-9262-27AB6E049F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -609,10 +609,10 @@
     <t>SeparateProducts</t>
   </si>
   <si>
-    <t>{\Wproduct\W:\W((\w+\s*\W)+)}</t>
-  </si>
-  <si>
     <t>{\Wproduct\W:\W(\d+\s*)+\W}</t>
+  </si>
+  <si>
+    <t>{\Wproduct\W:\W(.+)\W}</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,10 +1587,10 @@
         <v>190</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
live proving changes for saving in date received folder
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20BD4E-A035-4742-9262-27AB6E049F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD91D4D-BDB8-47A4-A575-F948342CCFB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17325" yWindow="3825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
     <t>{\Wproduct\W:\W(\d+\s*)+\W}</t>
   </si>
   <si>
-    <t>{\Wproduct\W:\W(.+)\W}</t>
+    <t>{\W{0,2}product\W{0,2}:\W{0,2}([^(},{)]+)</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes for address label regex, new logic for multi certs connected up
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD91D4D-BDB8-47A4-A575-F948342CCFB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704A661-256C-4B8B-80C8-3F81222AC282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17325" yWindow="3825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -613,6 +613,18 @@
   </si>
   <si>
     <t>{\W{0,2}product\W{0,2}:\W{0,2}([^(},{)]+)</t>
+  </si>
+  <si>
+    <t>AddressContinueRegex</t>
+  </si>
+  <si>
+    <t>\WContinue\W:(\w+)</t>
+  </si>
+  <si>
+    <t>AddressRegex</t>
+  </si>
+  <si>
+    <t>IN_strAddressLabel\W{0,2}:\W{0,2}(.+)",</t>
   </si>
 </sst>
 </file>
@@ -769,8 +781,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C54" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="6"/>
@@ -1089,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1606,20 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+      <c r="A54" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes for making ie full screen at log in and adding trd to address label
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704A661-256C-4B8B-80C8-3F81222AC282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03C0F44-B1BA-4865-AE8A-556E6ED91A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1167,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>34</v>
@@ -1178,7 +1178,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
changes for char limit, and fixing certificate logic
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03C0F44-B1BA-4865-AE8A-556E6ED91A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC91D5C-FAA9-40EA-AFE7-3F861C85333F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1156,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Trader changed to Edge
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC91D5C-FAA9-40EA-AFE7-3F861C85333F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DA5A39-0FC5-45EC-A6C2-059109263FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>36</v>
@@ -1200,7 +1200,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>37</v>
@@ -1211,7 +1211,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Recompile for issue with 1.0.48
</commit_message>
<xml_diff>
--- a/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
+++ b/rpa-certificates-of-free-sale/Documents/LiveConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-certificates-of-free-sale\rpa-certificates-of-free-sale\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/jason_savory_defra_gov_uk/Documents/Jason - In Progress Work/rpa-certificates-of-free-sale/rpa-certificates-of-free-sale/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DA5A39-0FC5-45EC-A6C2-059109263FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{84DA5A39-0FC5-45EC-A6C2-059109263FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C51386-A9C2-4BCB-8084-B6DD3301CEC0}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="690" windowWidth="20325" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Url for Trader CRM</t>
   </si>
   <si>
-    <t>C:\Users\{0}\Desktop\CoFS Logs_{1}.xlsx</t>
-  </si>
-  <si>
     <t>RobotWorkingFolder</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>IN_strAddressLabel\W{0,2}:\W{0,2}(.+)",</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\CoFS Logs_{1}.csv</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,7 +1141,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1237,13 +1237,13 @@
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>42</v>
@@ -1351,7 +1351,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>196</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>6</v>
@@ -1359,76 +1359,76 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1438,155 +1438,155 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,29 +1596,29 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1658,401 +1658,401 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" s="4"/>
     </row>

</xml_diff>